<commit_message>
Re-drew figures to be easier to read and be viewable in black and white
</commit_message>
<xml_diff>
--- a/hoomd_kvm_updated.xlsx
+++ b/hoomd_kvm_updated.xlsx
@@ -12,12 +12,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -195,34 +190,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>HOOMD GPUDirect Performance, 256K Lennard-Jones</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Simulation</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t> </a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -373,7 +341,7 @@
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:prstDash val="sysDash"/>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -442,7 +410,7 @@
                   <a:lumOff val="40000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:prstDash val="sysDot"/>
+              <a:prstDash val="dashDot"/>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -506,11 +474,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="112187264"/>
-        <c:axId val="112189824"/>
+        <c:axId val="120559104"/>
+        <c:axId val="120569856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="112187264"/>
+        <c:axId val="120559104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -541,13 +509,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112189824"/>
+        <c:crossAx val="120569856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="112189824"/>
+        <c:axId val="120569856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="200"/>
@@ -578,7 +546,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112187264"/>
+        <c:crossAx val="120559104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -733,11 +701,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="140404224"/>
-        <c:axId val="140405760"/>
+        <c:axId val="120915072"/>
+        <c:axId val="120916608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="140404224"/>
+        <c:axId val="120915072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -747,7 +715,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140405760"/>
+        <c:crossAx val="120916608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -755,7 +723,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140405760"/>
+        <c:axId val="120916608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.95"/>
@@ -767,7 +735,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140404224"/>
+        <c:crossAx val="120915072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1083,11 +1051,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145286656"/>
-        <c:axId val="145289216"/>
+        <c:axId val="121005184"/>
+        <c:axId val="121007488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145286656"/>
+        <c:axId val="121005184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -1117,13 +1085,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145289216"/>
+        <c:crossAx val="121007488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145289216"/>
+        <c:axId val="121007488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1152,7 +1120,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145286656"/>
+        <c:crossAx val="121005184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1199,7 +1167,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662883" cy="6292062"/>
+    <xdr:ext cx="8639236" cy="6279220"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2644,11 +2612,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Redrew the graphs again with different markers and lines.  Looks, better, but now the lines are too small to read/see.
</commit_message>
<xml_diff>
--- a/hoomd_kvm_updated.xlsx
+++ b/hoomd_kvm_updated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="270" windowWidth="22065" windowHeight="17040" tabRatio="500"/>
+    <workbookView xWindow="615" yWindow="285" windowWidth="22065" windowHeight="17040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="HOOMD" sheetId="2" r:id="rId1"/>
@@ -203,7 +203,7 @@
             <c:v>VM GPUDirect</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="sq">
+            <a:ln w="25400" cap="sq">
               <a:solidFill>
                 <a:schemeClr val="accent2">
                   <a:lumMod val="50000"/>
@@ -213,16 +213,16 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="8"/>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln>
-                <a:noFill/>
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
               </a:ln>
             </c:spPr>
           </c:marker>
@@ -271,7 +271,7 @@
             <c:v>VM No GPUDirect</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="sq">
+            <a:ln w="25400" cap="sq">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -279,14 +279,14 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="5"/>
+            <c:symbol val="plus"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln>
-                <a:noFill/>
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
               </a:ln>
             </c:spPr>
           </c:marker>
@@ -335,7 +335,7 @@
             <c:v>Base GPUDirect</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100">
+            <a:ln w="25400">
               <a:solidFill>
                 <a:schemeClr val="accent1">
                   <a:lumMod val="75000"/>
@@ -345,16 +345,16 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="8"/>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln>
-                <a:noFill/>
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
               </a:ln>
             </c:spPr>
           </c:marker>
@@ -403,7 +403,7 @@
             <c:v>Base No GPUDirect</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100">
+            <a:ln w="25400">
               <a:solidFill>
                 <a:schemeClr val="tx2">
                   <a:lumMod val="60000"/>
@@ -414,17 +414,17 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln>
-                <a:noFill/>
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
               </a:ln>
             </c:spPr>
           </c:marker>
@@ -474,11 +474,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="130509440"/>
-        <c:axId val="130512000"/>
+        <c:axId val="131404544"/>
+        <c:axId val="131406848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="130509440"/>
+        <c:axId val="131404544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -509,13 +509,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130512000"/>
+        <c:crossAx val="131406848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130512000"/>
+        <c:axId val="131406848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="200"/>
@@ -546,7 +546,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130509440"/>
+        <c:crossAx val="131404544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -715,11 +715,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="133343488"/>
-        <c:axId val="133353472"/>
+        <c:axId val="136331264"/>
+        <c:axId val="136332800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133343488"/>
+        <c:axId val="136331264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -729,7 +729,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133353472"/>
+        <c:crossAx val="136332800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -737,7 +737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133353472"/>
+        <c:axId val="136332800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.95"/>
@@ -749,7 +749,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133343488"/>
+        <c:crossAx val="136331264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1064,11 +1064,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133441792"/>
-        <c:axId val="133444352"/>
+        <c:axId val="136372224"/>
+        <c:axId val="136374528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133441792"/>
+        <c:axId val="136372224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -1098,13 +1098,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133444352"/>
+        <c:crossAx val="136374528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133444352"/>
+        <c:axId val="136374528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1133,7 +1133,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133441792"/>
+        <c:crossAx val="136372224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>

<commit_message>
Enlarged line sizes a bit for all images. Time to check if it fits
</commit_message>
<xml_diff>
--- a/hoomd_kvm_updated.xlsx
+++ b/hoomd_kvm_updated.xlsx
@@ -203,7 +203,7 @@
             <c:v>VM GPUDirect</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="sq">
+            <a:ln w="38100" cap="sq">
               <a:solidFill>
                 <a:schemeClr val="accent2">
                   <a:lumMod val="50000"/>
@@ -214,10 +214,10 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="x"/>
-            <c:size val="6"/>
+            <c:size val="9"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln>
+              <a:ln w="12700">
                 <a:solidFill>
                   <a:schemeClr val="accent2">
                     <a:lumMod val="50000"/>
@@ -271,7 +271,7 @@
             <c:v>VM No GPUDirect</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="sq">
+            <a:ln w="44450" cap="sq">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -280,10 +280,10 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="plus"/>
-            <c:size val="6"/>
+            <c:size val="9"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln>
+              <a:ln w="12700">
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
@@ -335,7 +335,7 @@
             <c:v>Base GPUDirect</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400">
+            <a:ln w="44450">
               <a:solidFill>
                 <a:schemeClr val="accent1">
                   <a:lumMod val="75000"/>
@@ -346,10 +346,10 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="diamond"/>
-            <c:size val="6"/>
+            <c:size val="9"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln>
+              <a:ln w="12700">
                 <a:solidFill>
                   <a:schemeClr val="accent1">
                     <a:lumMod val="75000"/>
@@ -403,7 +403,7 @@
             <c:v>Base No GPUDirect</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400">
+            <a:ln w="44450">
               <a:solidFill>
                 <a:schemeClr val="tx2">
                   <a:lumMod val="60000"/>
@@ -415,10 +415,10 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="square"/>
-            <c:size val="6"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln>
+              <a:ln w="12700">
                 <a:solidFill>
                   <a:schemeClr val="tx2">
                     <a:lumMod val="60000"/>

</xml_diff>